<commit_message>
now the Dates.csv table can add new events with some blank columns. NEED TO AT LEAST have eventid, event, first, and last day filled out.
</commit_message>
<xml_diff>
--- a/DevNotes/PMI Provided Course List Edits.xlsx
+++ b/DevNotes/PMI Provided Course List Edits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\SchedulePro\DevNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79F49AF-BAE5-4C54-8208-94C58E726D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ECC97B-FA71-44CA-9FA1-57E8D7D69537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2145" yWindow="0" windowWidth="28770" windowHeight="15270" tabRatio="882" firstSheet="2" activeTab="11" xr2:uid="{E7EE0092-2BA9-4A50-8785-723FB1934021}"/>
   </bookViews>
@@ -2138,7 +2138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2149,6 +2149,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2476,7 +2482,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="263">
+  <cellXfs count="264">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3122,6 +3128,7 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -19482,7 +19489,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19533,7 +19540,7 @@
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="263" t="s">
         <v>519</v>
       </c>
     </row>

</xml_diff>

<commit_message>
second export button added to also export event id and room id, this will help later in importing room numbers etc
</commit_message>
<xml_diff>
--- a/DevNotes/PMI Provided Course List Edits.xlsx
+++ b/DevNotes/PMI Provided Course List Edits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\SchedulePro\DevNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ECC97B-FA71-44CA-9FA1-57E8D7D69537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AAA972-C59A-44CC-AD2F-6417485B7F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="0" windowWidth="28770" windowHeight="15270" tabRatio="882" firstSheet="2" activeTab="11" xr2:uid="{E7EE0092-2BA9-4A50-8785-723FB1934021}"/>
+    <workbookView xWindow="-56430" yWindow="1290" windowWidth="20130" windowHeight="13500" tabRatio="882" firstSheet="2" activeTab="11" xr2:uid="{E7EE0092-2BA9-4A50-8785-723FB1934021}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Data" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5092" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5096" uniqueCount="526">
   <si>
     <t>Month</t>
   </si>
@@ -2023,6 +2023,18 @@
   </si>
   <si>
     <t>Instructor names corrected</t>
+  </si>
+  <si>
+    <t>Klaus has a course ID identical for 2 different courses</t>
+  </si>
+  <si>
+    <t>Oscar's name is wrong</t>
+  </si>
+  <si>
+    <t>Added TBD2,3 for Scott since can't have same courseid</t>
+  </si>
+  <si>
+    <t>added New1, New2 for Ori as above</t>
   </si>
 </sst>
 </file>
@@ -19486,10 +19498,10 @@
   <sheetPr codeName="Sheet12">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19552,6 +19564,26 @@
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>521</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>